<commit_message>
TT urban facility output updates
</commit_message>
<xml_diff>
--- a/output/Transitions Rule/summary_tables/transition_rule_summary_tables_Linde-Whiting.xlsx
+++ b/output/Transitions Rule/summary_tables/transition_rule_summary_tables_Linde-Whiting.xlsx
@@ -18,10 +18,10 @@
     <t xml:space="preserve">Variable</t>
   </si>
   <si>
-    <t xml:space="preserve">Rural Areas (National Average)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rural Areas (State Average)</t>
+    <t xml:space="preserve">National Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average</t>
   </si>
   <si>
     <t xml:space="preserve">Within 1 mile of HFC production facility</t>
@@ -63,10 +63,10 @@
     <t xml:space="preserve">Total Respiratory (hazard quotient)</t>
   </si>
   <si>
-    <t xml:space="preserve">Rural Areas (National Average) SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rural Areas (State Average) SD</t>
+    <t xml:space="preserve">National Average SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average SD</t>
   </si>
   <si>
     <t xml:space="preserve">Within 1 mile of HFC production facility SD</t>
@@ -438,22 +438,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C2" t="n">
-        <v>94</v>
-      </c>
-      <c r="D2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G2" t="e">
-        <v>#NUM!</v>
+        <v>83</v>
+      </c>
+      <c r="D2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E2" t="n">
+        <v>35</v>
+      </c>
+      <c r="F2" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="3">
@@ -461,22 +461,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>7.6</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G3" t="e">
-        <v>#NUM!</v>
+        <v>9.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>35</v>
+      </c>
+      <c r="E3" t="n">
+        <v>29</v>
+      </c>
+      <c r="F3" t="n">
+        <v>32</v>
+      </c>
+      <c r="G3" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="4">
@@ -484,22 +484,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>8.2</v>
+        <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="D4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G4" t="e">
-        <v>#NUM!</v>
+        <v>7.3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>43</v>
+      </c>
+      <c r="E4" t="n">
+        <v>36</v>
+      </c>
+      <c r="F4" t="n">
+        <v>22</v>
+      </c>
+      <c r="G4" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -507,22 +507,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C5" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="D5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G5" t="e">
-        <v>#NUM!</v>
+        <v>6.9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>61</v>
+      </c>
+      <c r="E5" t="n">
+        <v>49</v>
+      </c>
+      <c r="F5" t="n">
+        <v>38</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -530,22 +530,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C6" t="n">
-        <v>66</v>
-      </c>
-      <c r="D6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G6" t="e">
-        <v>#NUM!</v>
+        <v>62</v>
+      </c>
+      <c r="D6" t="n">
+        <v>34</v>
+      </c>
+      <c r="E6" t="n">
+        <v>39</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45</v>
+      </c>
+      <c r="G6" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="7">
@@ -553,22 +553,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>6.8</v>
+        <v>7.3</v>
       </c>
       <c r="C7" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="D7" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E7" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F7" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G7" t="e">
-        <v>#NUM!</v>
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>17</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" t="n">
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -576,22 +576,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>5.1</v>
+        <v>5.8</v>
       </c>
       <c r="C8" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="D8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G8" t="e">
-        <v>#NUM!</v>
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -599,22 +599,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
-      </c>
-      <c r="D9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G9" t="e">
-        <v>#NUM!</v>
+        <v>23</v>
+      </c>
+      <c r="D9" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" t="n">
+        <v>30</v>
+      </c>
+      <c r="F9" t="n">
+        <v>30</v>
+      </c>
+      <c r="G9" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -622,22 +622,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>0.32</v>
+        <v>0.37</v>
       </c>
       <c r="C10" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="D10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G10" t="e">
-        <v>#NUM!</v>
+        <v>0.3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.37</v>
       </c>
     </row>
   </sheetData>
@@ -682,22 +682,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C2" t="n">
-        <v>6.9</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -705,22 +705,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C3" t="n">
-        <v>4.3</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
@@ -728,22 +728,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>4.6</v>
+        <v>8.9</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -751,22 +751,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C5" t="n">
-        <v>5.5</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -774,22 +774,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" t="n">
+        <v>13</v>
+      </c>
+      <c r="F6" t="n">
+        <v>15</v>
+      </c>
+      <c r="G6" t="n">
         <v>19</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -797,22 +797,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>7.6</v>
+        <v>8.7</v>
       </c>
       <c r="C7" t="n">
-        <v>5.9</v>
+        <v>8.4</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>9.4</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>9.7</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -820,22 +820,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>6.4</v>
+        <v>7.8</v>
       </c>
       <c r="C8" t="n">
-        <v>4.6</v>
+        <v>8.4</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -843,10 +843,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>2.9</v>
+        <v>4.7</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -858,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="10">
@@ -869,19 +869,19 @@
         <v>0.14</v>
       </c>
       <c r="C10" t="n">
-        <v>0.051</v>
+        <v>0.058</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.022</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>